<commit_message>
Updated data in test data
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="19140" windowHeight="3885"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="19140" windowHeight="3885" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -107,12 +107,6 @@
     <t>testing</t>
   </si>
   <si>
-    <t>amuthan</t>
-  </si>
-  <si>
-    <t>sakthivel</t>
-  </si>
-  <si>
     <t>postProductWithPojo</t>
   </si>
   <si>
@@ -138,6 +132,12 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Manjeet</t>
+  </si>
+  <si>
+    <t>Singh</t>
   </si>
 </sst>
 </file>
@@ -486,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -541,7 +541,7 @@
         <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
@@ -558,7 +558,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
@@ -569,13 +569,13 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D5" s="3">
         <v>1</v>
@@ -586,13 +586,13 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
         <v>38</v>
-      </c>
-      <c r="C6" t="s">
-        <v>40</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>5</v>
@@ -610,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -800,30 +800,30 @@
         <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="G8" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" t="s">
         <v>32</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" t="s">
-        <v>34</v>
       </c>
       <c r="G9" t="s">
         <v>29</v>
@@ -831,7 +831,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
@@ -846,30 +846,30 @@
         <v>20</v>
       </c>
       <c r="F10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>20</v>

</xml_diff>